<commit_message>
att excel dia 03/01
</commit_message>
<xml_diff>
--- a/primeirasemanasetembro.xlsx
+++ b/primeirasemanasetembro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivina\Desktop\jogodobicho\jogodobicho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990A347F-B802-4738-83DB-02A4C626BE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BE2E18-B37F-42A8-ABB7-A6DAEB70A3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{500AFD6E-13E7-4543-8FDB-D63E104D29D0}"/>
   </bookViews>
@@ -539,16 +539,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6185FBA4-3391-45B3-811A-4861B6CE3709}">
-  <dimension ref="A1:T2081"/>
+  <dimension ref="A1:T2111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2055" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F2072" sqref="F2072"/>
+    <sheetView tabSelected="1" topLeftCell="A2083" zoomScale="88" workbookViewId="0">
+      <selection activeCell="I2107" sqref="I2107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
     <col min="8" max="8" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -36723,6 +36723,516 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2082" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2082">
+        <v>105</v>
+      </c>
+      <c r="B2082" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2082">
+        <v>0</v>
+      </c>
+      <c r="D2082">
+        <v>6461</v>
+      </c>
+      <c r="E2082">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2083" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2083">
+        <v>105</v>
+      </c>
+      <c r="B2083" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2083">
+        <v>0</v>
+      </c>
+      <c r="D2083">
+        <v>5211</v>
+      </c>
+      <c r="E2083">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2084" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2084">
+        <v>105</v>
+      </c>
+      <c r="B2084" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2084">
+        <v>0</v>
+      </c>
+      <c r="D2084">
+        <v>9028</v>
+      </c>
+      <c r="E2084">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2085" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2085">
+        <v>105</v>
+      </c>
+      <c r="B2085" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2085">
+        <v>0</v>
+      </c>
+      <c r="D2085">
+        <v>2117</v>
+      </c>
+      <c r="E2085">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2086" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2086">
+        <v>105</v>
+      </c>
+      <c r="B2086" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2086">
+        <v>0</v>
+      </c>
+      <c r="D2086">
+        <v>2013</v>
+      </c>
+      <c r="E2086">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2087" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2087">
+        <v>105</v>
+      </c>
+      <c r="B2087" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2087">
+        <v>0</v>
+      </c>
+      <c r="D2087">
+        <v>7895</v>
+      </c>
+      <c r="E2087">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2088" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2088">
+        <v>105</v>
+      </c>
+      <c r="B2088" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2088">
+        <v>0</v>
+      </c>
+      <c r="D2088">
+        <v>6400</v>
+      </c>
+      <c r="E2088">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2089" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2089">
+        <v>105</v>
+      </c>
+      <c r="B2089" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2089">
+        <v>0</v>
+      </c>
+      <c r="D2089">
+        <v>3594</v>
+      </c>
+      <c r="E2089">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2090" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2090">
+        <v>105</v>
+      </c>
+      <c r="B2090" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2090">
+        <v>0</v>
+      </c>
+      <c r="D2090">
+        <v>4779</v>
+      </c>
+      <c r="E2090">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2091" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2091">
+        <v>105</v>
+      </c>
+      <c r="B2091" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2091">
+        <v>0</v>
+      </c>
+      <c r="D2091">
+        <v>2595</v>
+      </c>
+      <c r="E2091">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2092" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2092">
+        <v>105</v>
+      </c>
+      <c r="B2092" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2092">
+        <v>1</v>
+      </c>
+      <c r="D2092">
+        <v>1876</v>
+      </c>
+      <c r="E2092">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2093" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2093">
+        <v>105</v>
+      </c>
+      <c r="B2093" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2093">
+        <v>1</v>
+      </c>
+      <c r="D2093">
+        <v>52</v>
+      </c>
+      <c r="E2093">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2094" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2094">
+        <v>105</v>
+      </c>
+      <c r="B2094" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2094">
+        <v>1</v>
+      </c>
+      <c r="D2094">
+        <v>7835</v>
+      </c>
+      <c r="E2094">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2095" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2095">
+        <v>105</v>
+      </c>
+      <c r="B2095" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2095">
+        <v>1</v>
+      </c>
+      <c r="D2095">
+        <v>9515</v>
+      </c>
+      <c r="E2095">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2096" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2096">
+        <v>105</v>
+      </c>
+      <c r="B2096" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2096">
+        <v>1</v>
+      </c>
+      <c r="D2096">
+        <v>3918</v>
+      </c>
+      <c r="E2096">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2097" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2097">
+        <v>105</v>
+      </c>
+      <c r="B2097" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2097">
+        <v>1</v>
+      </c>
+      <c r="D2097">
+        <v>7555</v>
+      </c>
+      <c r="E2097">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2098" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2098">
+        <v>105</v>
+      </c>
+      <c r="B2098" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2098">
+        <v>1</v>
+      </c>
+      <c r="D2098">
+        <v>4510</v>
+      </c>
+      <c r="E2098">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2099" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2099">
+        <v>105</v>
+      </c>
+      <c r="B2099" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2099">
+        <v>1</v>
+      </c>
+      <c r="D2099">
+        <v>763</v>
+      </c>
+      <c r="E2099">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2100">
+        <v>105</v>
+      </c>
+      <c r="B2100" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2100">
+        <v>1</v>
+      </c>
+      <c r="D2100">
+        <v>2835</v>
+      </c>
+      <c r="E2100">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2101">
+        <v>105</v>
+      </c>
+      <c r="B2101" s="10">
+        <v>46024</v>
+      </c>
+      <c r="C2101">
+        <v>1</v>
+      </c>
+      <c r="D2101">
+        <v>7052</v>
+      </c>
+      <c r="E2101">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2102">
+        <v>106</v>
+      </c>
+      <c r="B2102" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2102">
+        <v>0</v>
+      </c>
+      <c r="D2102">
+        <v>992</v>
+      </c>
+      <c r="E2102">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2103">
+        <v>106</v>
+      </c>
+      <c r="B2103" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2103">
+        <v>0</v>
+      </c>
+      <c r="D2103">
+        <v>541</v>
+      </c>
+      <c r="E2103">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2104">
+        <v>106</v>
+      </c>
+      <c r="B2104" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2104">
+        <v>0</v>
+      </c>
+      <c r="D2104">
+        <v>4001</v>
+      </c>
+      <c r="E2104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2105">
+        <v>106</v>
+      </c>
+      <c r="B2105" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2105">
+        <v>0</v>
+      </c>
+      <c r="D2105">
+        <v>3899</v>
+      </c>
+      <c r="E2105">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2106">
+        <v>106</v>
+      </c>
+      <c r="B2106" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2106">
+        <v>0</v>
+      </c>
+      <c r="D2106">
+        <v>761</v>
+      </c>
+      <c r="E2106">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2107">
+        <v>106</v>
+      </c>
+      <c r="B2107" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2107">
+        <v>0</v>
+      </c>
+      <c r="D2107">
+        <v>3501</v>
+      </c>
+      <c r="E2107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2108">
+        <v>106</v>
+      </c>
+      <c r="B2108" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2108">
+        <v>0</v>
+      </c>
+      <c r="D2108">
+        <v>9297</v>
+      </c>
+      <c r="E2108">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2109">
+        <v>106</v>
+      </c>
+      <c r="B2109" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2109">
+        <v>0</v>
+      </c>
+      <c r="D2109">
+        <v>1241</v>
+      </c>
+      <c r="E2109">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2110">
+        <v>106</v>
+      </c>
+      <c r="B2110" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2110">
+        <v>0</v>
+      </c>
+      <c r="D2110">
+        <v>6868</v>
+      </c>
+      <c r="E2110">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2111">
+        <v>106</v>
+      </c>
+      <c r="B2111" s="10">
+        <v>46025</v>
+      </c>
+      <c r="C2111">
+        <v>0</v>
+      </c>
+      <c r="D2111">
+        <v>144</v>
+      </c>
+      <c r="E2111">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>